<commit_message>
using CMake for raylib + raylib-cpp
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -16,13 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Theme:</t>
   </si>
   <si>
-    <t xml:space="preserve">Text adventure style game using raylib
-Inspired by the Fear and Hunger video game franchise</t>
+    <t xml:space="preserve">Text adventure engine via raylib-cpp</t>
   </si>
   <si>
     <t>Type</t>
@@ -58,15 +57,18 @@
     <t xml:space="preserve">Setup a dev env for raylib and cpp</t>
   </si>
   <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decide on game genre, concept, resources, and functions</t>
+  </si>
+  <si>
     <t>TODO</t>
   </si>
   <si>
-    <t>Game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decide on game genre, concept, resources, and functions</t>
-  </si>
-  <si>
     <t>Engine</t>
   </si>
   <si>
@@ -76,7 +78,10 @@
     <t xml:space="preserve">Display ttf font in the window</t>
   </si>
   <si>
-    <t xml:space="preserve">JRPG text animation</t>
+    <t xml:space="preserve">Revealing text animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse input</t>
   </si>
   <si>
     <t xml:space="preserve">Keyboard input</t>
@@ -89,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -148,8 +153,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +210,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor theme="4" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -262,7 +279,7 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
@@ -276,6 +293,7 @@
     <xf fontId="8" fillId="5" borderId="5" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
     <xf fontId="0" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="9" fillId="10" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -309,23 +327,23 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="3" fillId="6" borderId="0" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="9" fillId="10" borderId="0" numFmtId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="3" fillId="9" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="7" fillId="7" borderId="0" numFmtId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="3" fillId="9" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -339,6 +357,7 @@
     <cellStyle name="Heading 2" xfId="10" builtinId="17"/>
     <cellStyle name="40% - Accent5" xfId="11" builtinId="47"/>
     <cellStyle name="60% - Accent1" xfId="12" builtinId="32"/>
+    <cellStyle name="Good" xfId="13" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -906,106 +925,120 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>2</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" ht="28.5">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>3</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>13</v>
+      <c r="D7" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>13</v>
+      <c r="D8" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="12">
-        <v>2</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="13">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="14">
-        <v>3</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="11" t="s">
-        <v>16</v>
+      <c r="A11" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>13</v>
+      <c r="D11" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>21</v>
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>13</v>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A5:D6" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="C5:C6"/>
+  <sortState ref="A5:D7" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="C5:C7"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
added external library raygui
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -3,11 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$F$4</definedName>
+  </definedNames>
   <calcPr/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
@@ -16,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Theme:</t>
   </si>
@@ -24,6 +28,16 @@
     <t xml:space="preserve">Text adventure engine via raylib-cpp</t>
   </si>
   <si>
+    <t xml:space="preserve">End goal:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The engine will have implementations for these behaviours (its more like an API): 
+- Display text from a file (nicely) on screen depending on selected story event.
+- UI generation of choice event buttons depending on story event.
+- Implementation of "choices-matter" effect, changing story events based on choice events
+- Inventory system for choice complexity and immersion</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -42,6 +56,30 @@
     <t>Note</t>
   </si>
   <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create window</t>
+  </si>
+  <si>
+    <t>Dialogue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter by letter (LBL) animation for displaying text</t>
+  </si>
+  <si>
+    <t>https://www.raylib.com/examples/text/loader.html?name=text_writing_anim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design and implement dialogue nodes for a branch-style narrative</t>
+  </si>
+  <si>
+    <t>https://peerdh.com/blogs/programming-insights/building-an-interactive-narrative-engine-for-video-games</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit choices depending on inventory state </t>
+  </si>
+  <si>
     <t>Docs</t>
   </si>
   <si>
@@ -51,50 +89,41 @@
     <t>ONGOING</t>
   </si>
   <si>
+    <t xml:space="preserve">Design the games basic concepts that will be implemented in the future</t>
+  </si>
+  <si>
     <t>Env</t>
   </si>
   <si>
     <t xml:space="preserve">Setup a dev env for raylib and cpp</t>
   </si>
   <si>
-    <t>COMPLETED</t>
-  </si>
-  <si>
-    <t>Game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decide on game genre, concept, resources, and functions</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Engine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create new, resizable window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display ttf font in the window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revealing text animation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mouse input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyboard input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modularize the story text into files</t>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design and implement states for game narrative</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seperate the main surface into parts: Story, Choices, Inventory, Status, Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement drawing text for the story system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement showing choices dep. on dialogue node </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -159,8 +188,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11.000000"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +251,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
       </patternFill>
     </fill>
   </fills>
@@ -279,7 +326,7 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
@@ -294,23 +341,25 @@
     <xf fontId="0" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="9" fillId="10" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="3" fillId="12" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="4" numFmtId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,31 +368,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="3" fillId="6" borderId="0" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="9" fillId="10" borderId="0" numFmtId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="3" fillId="9" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="7" fillId="7" borderId="0" numFmtId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="16">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -358,6 +407,8 @@
     <cellStyle name="40% - Accent5" xfId="11" builtinId="47"/>
     <cellStyle name="60% - Accent1" xfId="12" builtinId="32"/>
     <cellStyle name="Good" xfId="13" builtinId="26"/>
+    <cellStyle name="20% - Accent5" xfId="14" builtinId="46"/>
+    <cellStyle name="Accent3" xfId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -859,187 +910,313 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="2" width="14.140625"/>
-    <col customWidth="1" min="2" max="2" style="3" width="33.7109375"/>
-    <col min="3" max="3" style="2" width="9.140625"/>
-    <col customWidth="1" min="4" max="4" style="2" width="11.57421875"/>
-    <col customWidth="1" min="5" max="5" width="37.00390625"/>
-    <col customWidth="1" min="6" max="6" style="1" width="25.28125"/>
-    <col min="7" max="16384" style="1" width="9.140625"/>
+    <col customWidth="1" min="2" max="2" width="59.421875"/>
   </cols>
   <sheetData>
-    <row r="1" ht="57">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="14.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+    </row>
+    <row r="2" ht="114">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" style="3" width="14.140625"/>
+    <col customWidth="1" min="2" max="2" style="4" width="37.57421875"/>
+    <col min="3" max="3" style="3" width="9.140625"/>
+    <col customWidth="1" min="4" max="4" style="3" width="11.57421875"/>
+    <col customWidth="1" min="5" max="5" style="5" width="37.00390625"/>
+    <col customWidth="1" min="6" max="6" style="4" width="58.00390625"/>
+    <col min="7" max="7" style="3" width="9.140625"/>
+    <col min="8" max="16384" style="3" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="6" customFormat="1" ht="15">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" s="6" customFormat="1" ht="15">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" ht="28.5">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" ht="28.5">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="11">
-        <v>2</v>
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>13</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" ht="28.5">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="13">
-        <v>3</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="11">
-        <v>2</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="13">
-        <v>3</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" ht="28.5">
+      <c r="A9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" ht="28.5">
+      <c r="A10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" ht="28.5">
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" ht="28.5">
+      <c r="A12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A5:D7" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="C5:C7"/>
+  <autoFilter ref="A1:F4">
+    <sortState ref="A1:A4">
+      <sortCondition descending="0" ref="A1:A4"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:F4" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A1:A3"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="F3"/>
+    <hyperlink r:id="rId2" ref="F4"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>

</xml_diff>

<commit_message>
simpler version done and running fine
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Description" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$F$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$F$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr/>
@@ -457,7 +457,7 @@
     <xf fontId="0" fillId="11" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="12" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -477,17 +477,11 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="4" fillId="0" borderId="4" numFmtId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="4" numFmtId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -510,14 +504,8 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="14" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1087,261 +1075,261 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="6" width="14.140625"/>
-    <col customWidth="1" min="2" max="2" style="7" width="37.57421875"/>
+    <col customWidth="1" min="2" max="2" style="5" width="37.57421875"/>
     <col min="3" max="3" style="6" width="9.140625"/>
     <col customWidth="1" min="4" max="4" style="6" width="11.57421875"/>
-    <col customWidth="1" min="5" max="5" style="7" width="37.00390625"/>
-    <col customWidth="1" min="6" max="6" style="7" width="58.00390625"/>
+    <col customWidth="1" min="5" max="5" style="5" width="37.00390625"/>
+    <col customWidth="1" min="6" max="6" style="5" width="58.00390625"/>
     <col min="7" max="16384" style="6" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" ht="15">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="7" customFormat="1" ht="15">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" ht="42.75">
-      <c r="A2" s="10" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" ht="42.75" hidden="1">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" ht="28.5">
-      <c r="A3" s="10" t="s">
+    <row r="3" ht="28.5" hidden="1">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>3</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" ht="28.5">
-      <c r="A4" s="10" t="s">
+    <row r="4" ht="28.5" hidden="1">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>2</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7"/>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" ht="42.75">
+    <row r="5" ht="42.75" hidden="1">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" ht="28.5">
+    <row r="6" ht="28.5" hidden="1">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" ht="57">
+    <row r="7" ht="57" hidden="1">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" ht="28.5">
-      <c r="A8" s="10" t="s">
+    <row r="8" ht="28.5" hidden="1">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>2</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="D8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" ht="42.75">
+    <row r="9" ht="42.75" hidden="1">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" ht="28.5">
+    <row r="10" ht="28.5" hidden="1">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" ht="28.5">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" ht="28.5" hidden="1">
       <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" ht="42.75">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" ht="42.75" hidden="1">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>3</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" ht="28.5">
-      <c r="A13" s="10" t="s">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" ht="28.5" hidden="1">
+      <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="16">
         <v>5</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" s="10" t="s">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" ht="14.25" hidden="1">
+      <c r="A14" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1350,14 +1338,14 @@
       <c r="C14" s="6">
         <v>0</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" s="10" t="s">
+      <c r="D14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" ht="14.25" hidden="1">
+      <c r="A15" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1366,12 +1354,12 @@
       <c r="C15" s="6">
         <v>0</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" s="10" t="s">
+      <c r="D15" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" hidden="1">
+      <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1380,12 +1368,12 @@
       <c r="C16" s="6">
         <v>0</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" s="10" t="s">
+      <c r="D16" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" hidden="1">
+      <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1394,151 +1382,151 @@
       <c r="C17" s="6">
         <v>0</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" ht="28.5">
-      <c r="A18" s="10" t="s">
+      <c r="D17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" ht="28.5" hidden="1">
+      <c r="A18" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="9">
         <v>1</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="20" t="s">
+      <c r="D18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" ht="14.25" hidden="1">
+      <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="12">
         <v>2</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="A20" s="10" t="s">
+      <c r="D19" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" hidden="1">
+      <c r="A20" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="12">
         <v>2</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" ht="28.5">
-      <c r="A21" s="10" t="s">
+      <c r="D20" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" ht="28.5" hidden="1">
+      <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="17">
         <v>4</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="20" t="s">
+      <c r="D21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" ht="28.5">
       <c r="A22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="9">
         <v>1</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="18"/>
+      <c r="D22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" ht="42.75">
-      <c r="A24" s="10" t="s">
+      <c r="D23" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" ht="42.75" hidden="1">
+      <c r="A24" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="9">
         <v>1</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="10" t="s">
+      <c r="D24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" ht="14.25" hidden="1">
+      <c r="A25" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="12">
         <v>2</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" ht="28.5">
+      <c r="D25" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" ht="28.5" hidden="1">
       <c r="A26" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="6">
         <v>0</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" ht="28.5">
+      <c r="D26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" ht="28.5" hidden="1">
       <c r="A27" s="6" t="s">
         <v>59</v>
       </c>
@@ -1548,16 +1536,16 @@
       <c r="C27" s="6">
         <v>0</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="20" t="s">
+      <c r="D27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" ht="28.5">
-      <c r="A28" s="10" t="s">
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" ht="28.5" hidden="1">
+      <c r="A28" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1566,12 +1554,12 @@
       <c r="C28" s="6">
         <v>0</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" ht="28.5">
-      <c r="A29" s="10" t="s">
+      <c r="D28" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" ht="28.5" hidden="1">
+      <c r="A29" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1580,12 +1568,12 @@
       <c r="C29" s="6">
         <v>0</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25">
-      <c r="A30" s="10" t="s">
+      <c r="D29" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" hidden="1">
+      <c r="A30" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1594,12 +1582,17 @@
       <c r="C30" s="6">
         <v>0</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="10" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="States"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A1:A30">
       <sortCondition descending="0" ref="A1:A30"/>
     </sortState>

</xml_diff>